<commit_message>
#430 Script generated from Expression is saved and added to the module
</commit_message>
<xml_diff>
--- a/dev/src/test/module/TestItemExcel.xlsx
+++ b/dev/src/test/module/TestItemExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dev\src\test\module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF2C160-A3D3-471B-9392-CB8EF03A9BCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26920F4-40AB-4951-80A0-FB9C98DA26A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5145" yWindow="2955" windowWidth="19695" windowHeight="11100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestItemExcel" sheetId="10" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
@@ -96,6 +96,42 @@
   </si>
   <si>
     <t>TestItemExcel_Details</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>expression</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>inputFields</t>
+  </si>
+  <si>
+    <t>loggerName</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>Period.between(DateOfBirth, LocalDate.now()).getYears()</t>
+  </si>
+  <si>
+    <t>java.time.Period,java.time.LocalDate</t>
+  </si>
+  <si>
+    <t>imports</t>
+  </si>
+  <si>
+    <t>TestItemExcel_DetailsAgeUpdateExpression</t>
   </si>
 </sst>
 </file>
@@ -276,7 +312,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,6 +519,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -771,7 +819,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -810,6 +858,14 @@
     </xf>
     <xf numFmtId="43" fontId="18" fillId="37" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1170,7 +1226,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A1:XFD1048576"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,10 +1375,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE06FA1-F234-41DF-B799-9E2CFD7178EC}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,36 +1386,44 @@
     <col min="1" max="1" width="11.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="40.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="15"/>
+    <col min="4" max="4" width="40.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="15"/>
+    <col min="10" max="10" width="22.5703125" style="23" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="23"/>
+    <col min="12" max="12" width="16.28515625" style="23" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" style="23" customWidth="1"/>
+    <col min="15" max="15" width="19.85546875" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="22" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="22" t="s">
         <v>10</v>
       </c>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
       <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="J1" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1369,35 +1433,44 @@
       <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>4</v>
       </c>
+      <c r="E2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H2" s="17" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="17" t="s">
         <v>12</v>
       </c>
+      <c r="J2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="25" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1405,19 +1478,14 @@
         <v>24</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="b">
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="16">
         <v>1</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="16">
-        <v>1</v>
-      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1427,11 +1495,11 @@
       <c r="C4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="15" t="b">
+      <c r="I4" s="15" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1442,11 +1510,53 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="23">
+        <v>0</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:L1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="J1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#430 make name, version and loggerName optional
</commit_message>
<xml_diff>
--- a/dev/src/test/module/TestItemExcel.xlsx
+++ b/dev/src/test/module/TestItemExcel.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t xml:space="preserve">xsd</t>
   </si>
@@ -98,16 +98,13 @@
     <t xml:space="preserve">multiplicity</t>
   </si>
   <si>
-    <t xml:space="preserve">version</t>
-  </si>
-  <si>
     <t xml:space="preserve">imports</t>
   </si>
   <si>
     <t xml:space="preserve">inputFields</t>
   </si>
   <si>
-    <t xml:space="preserve">loggerName</t>
+    <t xml:space="preserve">loggerPrefix</t>
   </si>
   <si>
     <t xml:space="preserve">TestItemExcel_Details</t>
@@ -134,16 +131,13 @@
     <t xml:space="preserve">integer</t>
   </si>
   <si>
-    <t xml:space="preserve">TestItemExcel_DetailsAgeUpdateExpression</t>
-  </si>
-  <si>
     <t xml:space="preserve">java.time.Period,java.time.LocalDate</t>
   </si>
   <si>
     <t xml:space="preserve">DateOfBirth,DateOfDeath</t>
   </si>
   <si>
-    <t xml:space="preserve">org.cristalise.dsl.test.TestItemExcel.DetailsAgeUpdateExpression</t>
+    <t xml:space="preserve">org.cristalise.devtest</t>
   </si>
   <si>
     <t xml:space="preserve">Period.between(DateOfBirth, DateOfDeath ?: LocalDate.now()).getYears()</t>
@@ -420,7 +414,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -671,10 +665,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:AMJ8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O15" activeCellId="0" sqref="O15"/>
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -689,13 +683,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="6.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="15.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="20" width="22.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="20" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="20" width="16.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="20" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="20" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="20" width="42.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="20" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="20" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="20" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="20" width="41.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="15" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -719,8 +712,8 @@
       <c r="L1" s="21"/>
       <c r="M1" s="21"/>
       <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
@@ -754,35 +747,31 @@
         <v>13</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="22" t="s">
         <v>23</v>
       </c>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="18" t="n">
         <v>1</v>
@@ -819,10 +808,10 @@
         <v>17</v>
       </c>
       <c r="B6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,13 +819,13 @@
         <v>17</v>
       </c>
       <c r="B7" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -844,35 +833,29 @@
         <v>17</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="K8" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="L8" s="23" t="s">
         <v>37</v>
-      </c>
-      <c r="L8" s="20" t="n">
-        <v>0</v>
       </c>
       <c r="M8" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="N8" s="20" t="s">
+      <c r="N8" s="23" t="s">
         <v>39</v>
-      </c>
-      <c r="O8" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="P8" s="23" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="K1:N1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>